<commit_message>
Se ajustan las instrucciones
</commit_message>
<xml_diff>
--- a/mensajes.xlsx
+++ b/mensajes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\sistemas\Descargas\alcaldiaBot\robotcito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\sistemas\Descargas\alcaldiaBot\wabot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -389,7 +389,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -443,5 +443,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se jsuta la plantilla de excel mensajes
</commit_message>
<xml_diff>
--- a/mensajes.xlsx
+++ b/mensajes.xlsx
@@ -33,9 +33,6 @@
     <t>https://puertolopez-meta.softwaretributario.com/impuestos.portal.wpnbienvenidoipu.aspx?IPU</t>
   </si>
   <si>
-    <t>Estimado(a) Servidor Público CORONADO BAQUERO MARCO ALBERTO, la Alcaldía Municipal de Puerto López lo invita a realizar el pago de las obligaciones del Impuesto Predial .Le recordamos que actualmente el acuerdo 015 de 2025 otorga un beneficio de descuento de intereses de hasta el 80%.  Consulte su estado de cuenta en:</t>
-  </si>
-  <si>
     <t>imagePath</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>archivos/archivo.pdf</t>
+  </si>
+  <si>
+    <t>Aquí va el mensaje personalizado</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -409,16 +409,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -426,19 +426,19 @@
         <v>3508207373</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>